<commit_message>
Removed unnecessary files and updated dema1/dema 1.xlsx
</commit_message>
<xml_diff>
--- a/dema1/dema 1.xlsx
+++ b/dema1/dema 1.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\dema1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Dema-Practical\dema1\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11490" windowHeight="4635"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11490" windowHeight="4635" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Q1" sheetId="1" r:id="rId1"/>
@@ -919,33 +919,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -980,6 +953,33 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1022,7 +1022,7 @@
         <xdr:cNvPr id="2" name="TextBox 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1357,7 +1357,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:M440"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
@@ -5053,14 +5053,14 @@
       <c r="F2" s="34"/>
       <c r="G2" s="35"/>
       <c r="H2" s="4"/>
-      <c r="K2" s="59" t="s">
+      <c r="K2" s="50" t="s">
         <v>81</v>
       </c>
-      <c r="L2" s="60"/>
-      <c r="M2" s="60"/>
-      <c r="N2" s="60"/>
-      <c r="O2" s="60"/>
-      <c r="P2" s="61"/>
+      <c r="L2" s="51"/>
+      <c r="M2" s="51"/>
+      <c r="N2" s="51"/>
+      <c r="O2" s="51"/>
+      <c r="P2" s="52"/>
     </row>
     <row r="3" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
@@ -5081,12 +5081,12 @@
       <c r="F3" s="34"/>
       <c r="G3" s="35"/>
       <c r="H3" s="4"/>
-      <c r="K3" s="62"/>
-      <c r="L3" s="63"/>
-      <c r="M3" s="63"/>
-      <c r="N3" s="63"/>
-      <c r="O3" s="63"/>
-      <c r="P3" s="64"/>
+      <c r="K3" s="53"/>
+      <c r="L3" s="54"/>
+      <c r="M3" s="54"/>
+      <c r="N3" s="54"/>
+      <c r="O3" s="54"/>
+      <c r="P3" s="55"/>
     </row>
     <row r="4" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
@@ -5107,16 +5107,16 @@
       <c r="F4" s="34"/>
       <c r="G4" s="35"/>
       <c r="H4" s="4"/>
-      <c r="K4" s="65" t="s">
+      <c r="K4" s="56" t="s">
         <v>78</v>
       </c>
-      <c r="L4" s="66"/>
-      <c r="M4" s="67"/>
-      <c r="N4" s="65" t="s">
+      <c r="L4" s="57"/>
+      <c r="M4" s="58"/>
+      <c r="N4" s="56" t="s">
         <v>84</v>
       </c>
-      <c r="O4" s="66"/>
-      <c r="P4" s="67"/>
+      <c r="O4" s="57"/>
+      <c r="P4" s="58"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
@@ -5137,16 +5137,16 @@
       <c r="F5" s="34"/>
       <c r="G5" s="35"/>
       <c r="H5" s="4"/>
-      <c r="K5" s="68" t="s">
+      <c r="K5" s="59" t="s">
         <v>86</v>
       </c>
-      <c r="L5" s="69"/>
-      <c r="M5" s="70"/>
-      <c r="N5" s="68">
+      <c r="L5" s="60"/>
+      <c r="M5" s="61"/>
+      <c r="N5" s="59">
         <v>5</v>
       </c>
-      <c r="O5" s="69"/>
-      <c r="P5" s="70"/>
+      <c r="O5" s="60"/>
+      <c r="P5" s="61"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
@@ -5227,11 +5227,11 @@
       <c r="F8" s="34"/>
       <c r="G8" s="35"/>
       <c r="H8" s="4"/>
-      <c r="K8" s="50" t="s">
+      <c r="K8" s="62" t="s">
         <v>92</v>
       </c>
-      <c r="L8" s="51"/>
-      <c r="M8" s="52"/>
+      <c r="L8" s="63"/>
+      <c r="M8" s="64"/>
       <c r="N8" s="47">
         <v>3.5</v>
       </c>
@@ -5257,16 +5257,16 @@
       <c r="F9" s="34"/>
       <c r="G9" s="35"/>
       <c r="H9" s="4"/>
-      <c r="K9" s="53" t="s">
+      <c r="K9" s="65" t="s">
         <v>94</v>
       </c>
-      <c r="L9" s="54"/>
-      <c r="M9" s="55"/>
-      <c r="N9" s="56">
+      <c r="L9" s="66"/>
+      <c r="M9" s="67"/>
+      <c r="N9" s="68">
         <v>3</v>
       </c>
-      <c r="O9" s="57"/>
-      <c r="P9" s="58"/>
+      <c r="O9" s="69"/>
+      <c r="P9" s="70"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
@@ -5570,6 +5570,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="K7:M7"/>
+    <mergeCell ref="N7:P7"/>
+    <mergeCell ref="K8:M8"/>
+    <mergeCell ref="N8:P8"/>
+    <mergeCell ref="K9:M9"/>
+    <mergeCell ref="N9:P9"/>
     <mergeCell ref="K6:M6"/>
     <mergeCell ref="N6:P6"/>
     <mergeCell ref="K2:P3"/>
@@ -5577,12 +5583,6 @@
     <mergeCell ref="N4:P4"/>
     <mergeCell ref="K5:M5"/>
     <mergeCell ref="N5:P5"/>
-    <mergeCell ref="K7:M7"/>
-    <mergeCell ref="N7:P7"/>
-    <mergeCell ref="K8:M8"/>
-    <mergeCell ref="N8:P8"/>
-    <mergeCell ref="K9:M9"/>
-    <mergeCell ref="N9:P9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7120,8 +7120,8 @@
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7170,11 +7170,23 @@
       <c r="A2" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
+      <c r="B2" s="28" t="str">
+        <f>LEFT(A2,SEARCH(" ",A2)-1)</f>
+        <v>Rohit</v>
+      </c>
+      <c r="C2" s="28" t="str">
+        <f>RIGHT(A2,LEN(A2)-SEARCH(" ",A2))</f>
+        <v>Gupta</v>
+      </c>
       <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
+      <c r="E2" s="28">
+        <f>LEN(A2)</f>
+        <v>11</v>
+      </c>
+      <c r="F2" s="28" t="str">
+        <f>TRIM(A2)</f>
+        <v>Rohit Gupta</v>
+      </c>
       <c r="G2" s="28"/>
       <c r="H2" s="28"/>
       <c r="I2" s="29"/>
@@ -7183,10 +7195,19 @@
       <c r="A3" s="36" t="s">
         <v>62</v>
       </c>
-      <c r="B3" s="28"/>
-      <c r="C3" s="28"/>
+      <c r="B3" s="28" t="str">
+        <f t="shared" ref="B3:B8" si="0">LEFT(A3,SEARCH(" ",A3)-1)</f>
+        <v>Sanjeev</v>
+      </c>
+      <c r="C3" s="28" t="str">
+        <f t="shared" ref="C3:C8" si="1">RIGHT(A3,LEN(A3)-SEARCH(" ",A3))</f>
+        <v>kumar</v>
+      </c>
       <c r="D3" s="28"/>
-      <c r="E3" s="28"/>
+      <c r="E3" s="28">
+        <f t="shared" ref="E3:E4" si="2">LEN(A3)</f>
+        <v>13</v>
+      </c>
       <c r="F3" s="28"/>
       <c r="G3" s="28"/>
       <c r="H3" s="28"/>
@@ -7196,10 +7217,19 @@
       <c r="A4" s="36" t="s">
         <v>63</v>
       </c>
-      <c r="B4" s="28"/>
+      <c r="B4" s="28" t="str">
+        <f t="shared" si="0"/>
+        <v>Rohit</v>
+      </c>
       <c r="C4" s="28"/>
-      <c r="D4" s="28"/>
-      <c r="E4" s="28"/>
+      <c r="D4" s="28" t="str">
+        <f>MID(A4,6,)</f>
+        <v/>
+      </c>
+      <c r="E4" s="28">
+        <f t="shared" si="2"/>
+        <v>17</v>
+      </c>
       <c r="F4" s="28"/>
       <c r="G4" s="28"/>
       <c r="H4" s="28"/>
@@ -7209,10 +7239,16 @@
       <c r="A5" s="36" t="s">
         <v>64</v>
       </c>
-      <c r="B5" s="28"/>
+      <c r="B5" s="28" t="str">
+        <f t="shared" si="0"/>
+        <v>Naveen</v>
+      </c>
       <c r="C5" s="28"/>
       <c r="D5" s="28"/>
-      <c r="E5" s="28"/>
+      <c r="E5" s="28">
+        <f>LEN(A5)</f>
+        <v>20</v>
+      </c>
       <c r="F5" s="28"/>
       <c r="G5" s="28"/>
       <c r="H5" s="28"/>
@@ -7222,10 +7258,16 @@
       <c r="A6" s="36" t="s">
         <v>65</v>
       </c>
-      <c r="B6" s="28"/>
+      <c r="B6" s="28" t="str">
+        <f t="shared" si="0"/>
+        <v>Arti</v>
+      </c>
       <c r="C6" s="28"/>
       <c r="D6" s="28"/>
-      <c r="E6" s="28"/>
+      <c r="E6" s="28">
+        <f t="shared" ref="E6:E8" si="3">LEN(A6)</f>
+        <v>18</v>
+      </c>
       <c r="F6" s="28"/>
       <c r="G6" s="28"/>
       <c r="H6" s="28"/>
@@ -7235,10 +7277,16 @@
       <c r="A7" s="36" t="s">
         <v>66</v>
       </c>
-      <c r="B7" s="28"/>
+      <c r="B7" s="28" t="str">
+        <f t="shared" si="0"/>
+        <v>Rohit</v>
+      </c>
       <c r="C7" s="28"/>
       <c r="D7" s="28"/>
-      <c r="E7" s="28"/>
+      <c r="E7" s="28">
+        <f t="shared" si="3"/>
+        <v>15</v>
+      </c>
       <c r="F7" s="28"/>
       <c r="G7" s="28"/>
       <c r="H7" s="28"/>
@@ -7248,10 +7296,16 @@
       <c r="A8" s="37" t="s">
         <v>67</v>
       </c>
-      <c r="B8" s="28"/>
+      <c r="B8" s="28" t="str">
+        <f t="shared" si="0"/>
+        <v>Rahul</v>
+      </c>
       <c r="C8" s="28"/>
       <c r="D8" s="28"/>
-      <c r="E8" s="28"/>
+      <c r="E8" s="28">
+        <f t="shared" si="3"/>
+        <v>17</v>
+      </c>
       <c r="F8" s="28"/>
       <c r="G8" s="28"/>
       <c r="H8" s="30"/>

</xml_diff>